<commit_message>
Added DB data import
</commit_message>
<xml_diff>
--- a/data/agri_production/cereals.xlsx
+++ b/data/agri_production/cereals.xlsx
@@ -341,8 +341,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>523126</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>178728</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
@@ -384,7 +384,7 @@
   <cols>
     <col min="1" max="1" width="19.921875" customWidth="true"/>
     <col min="4" max="4" width="39.3125" customWidth="true"/>
-    <col min="5" max="5" width="42.2890625" customWidth="true"/>
+    <col min="5" max="5" width="38.3125" customWidth="true"/>
     <col min="2" max="2" width="10.4921875" customWidth="true"/>
     <col min="3" max="3" width="17.25" customWidth="true"/>
   </cols>
@@ -392,7 +392,7 @@
     <row r="6">
       <c r="A6" s="14" t="inlineStr">
         <is>
-          <t>Crop production in EU standard humidity [APRO_CPSH1__custom_7737950]</t>
+          <t>Crop production in EU standard humidity [apro_cpsh1__custom_7891749]</t>
         </is>
       </c>
     </row>
@@ -428,7 +428,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>18/09/2023 23:00</t>
+          <t>13/10/2023 23:00</t>
         </is>
       </c>
     </row>
@@ -498,7 +498,7 @@
       </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>Harvested production in EU standard humidity (1000 t)</t>
+          <t>Area (cultivation/harvested/production) (1000 ha)</t>
         </is>
       </c>
     </row>
@@ -593,7 +593,7 @@
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>Harvested production in EU standard humidity (1000 t)</t>
+          <t>Area (cultivation/harvested/production) (1000 ha)</t>
         </is>
       </c>
     </row>
@@ -1097,7 +1097,7 @@
       </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>2013</t>
         </is>
       </c>
     </row>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="C49" s="16" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>2014</t>
         </is>
       </c>
     </row>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="C50" s="2" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2015</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="C51" s="16" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2016</t>
         </is>
       </c>
     </row>
@@ -1145,7 +1145,7 @@
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2017</t>
         </is>
       </c>
     </row>
@@ -1157,7 +1157,7 @@
       </c>
       <c r="C53" s="16" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
@@ -1169,7 +1169,7 @@
       </c>
       <c r="C54" s="2" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>2019</t>
         </is>
       </c>
     </row>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="C55" s="16" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>2020</t>
         </is>
       </c>
     </row>
@@ -1193,7 +1193,7 @@
       </c>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2021</t>
         </is>
       </c>
     </row>
@@ -1204,6 +1204,18 @@
         </is>
       </c>
       <c r="C57" s="16" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" s="2" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="C58" s="2" t="inlineStr">
         <is>
           <t>2023</t>
         </is>
@@ -1246,12 +1258,14 @@
     <col min="19" max="19" width="4.98046875" customWidth="true"/>
     <col min="20" max="20" width="9.9609375" customWidth="true"/>
     <col min="21" max="21" width="4.98046875" customWidth="true"/>
+    <col min="22" max="22" width="9.9609375" customWidth="true"/>
+    <col min="23" max="23" width="4.98046875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>Data extracted on 09/10/2023 11:29:41 from [ESTAT]</t>
+          <t>Data extracted on 17/10/2023 16:28:13 from [ESTAT]</t>
         </is>
       </c>
     </row>
@@ -1263,7 +1277,7 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>Crop production in EU standard humidity [APRO_CPSH1__custom_7737950]</t>
+          <t>Crop production in EU standard humidity [apro_cpsh1__custom_7891749]</t>
         </is>
       </c>
     </row>
@@ -1275,7 +1289,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>18/09/2023 23:00</t>
+          <t>13/10/2023 23:00</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1327,7 @@
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>Harvested production in EU standard humidity (1000 t)</t>
+          <t>Area (cultivation/harvested/production) (1000 ha)</t>
         </is>
       </c>
     </row>
@@ -1327,100 +1341,110 @@
       </c>
       <c r="B9" s="4" t="inlineStr">
         <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D9" s="4" t="inlineStr">
+        <is>
           <t>2014</t>
         </is>
       </c>
-      <c r="C9" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D9" s="4" t="inlineStr">
+      <c r="E9" s="4" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F9" s="4" t="inlineStr">
         <is>
           <t>2015</t>
         </is>
       </c>
-      <c r="E9" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="F9" s="4" t="inlineStr">
+      <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H9" s="4" t="inlineStr">
         <is>
           <t>2016</t>
         </is>
       </c>
-      <c r="G9" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H9" s="4" t="inlineStr">
+      <c r="I9" s="4" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J9" s="4" t="inlineStr">
         <is>
           <t>2017</t>
         </is>
       </c>
-      <c r="I9" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="J9" s="4" t="inlineStr">
+      <c r="K9" s="4" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="L9" s="4" t="inlineStr">
         <is>
           <t>2018</t>
         </is>
       </c>
-      <c r="K9" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="L9" s="4" t="inlineStr">
+      <c r="M9" s="4" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="N9" s="4" t="inlineStr">
         <is>
           <t>2019</t>
         </is>
       </c>
-      <c r="M9" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="N9" s="4" t="inlineStr">
+      <c r="O9" s="4" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P9" s="4" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
       </c>
-      <c r="O9" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P9" s="4" t="inlineStr">
+      <c r="Q9" s="4" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="R9" s="4" t="inlineStr">
         <is>
           <t>2021</t>
         </is>
       </c>
-      <c r="Q9" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="R9" s="4" t="inlineStr">
+      <c r="S9" s="4" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T9" s="4" t="inlineStr">
         <is>
           <t>2022</t>
         </is>
       </c>
-      <c r="S9" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="T9" s="4" t="inlineStr">
+      <c r="U9" s="4" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V9" s="4" t="inlineStr">
         <is>
           <t>2023</t>
         </is>
       </c>
-      <c r="U9" s="4" t="inlineStr">
+      <c r="W9" s="4" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -1532,6 +1556,16 @@
           <t/>
         </is>
       </c>
+      <c r="V10" s="9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W10" s="9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="8" t="inlineStr">
@@ -1540,15 +1574,17 @@
         </is>
       </c>
       <c r="B11" s="19" t="n">
-        <v>332329.17</v>
+        <v>57423.36</v>
       </c>
       <c r="C11" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="D11" s="19" t="n">
-        <v>316307.63</v>
+      <c r="D11" s="10" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
       </c>
       <c r="E11" s="10" t="inlineStr">
         <is>
@@ -1556,7 +1592,7 @@
         </is>
       </c>
       <c r="F11" s="19" t="n">
-        <v>301811.62</v>
+        <v>57571.74</v>
       </c>
       <c r="G11" s="10" t="inlineStr">
         <is>
@@ -1564,7 +1600,7 @@
         </is>
       </c>
       <c r="H11" s="19" t="n">
-        <v>309993.16</v>
+        <v>57220.53</v>
       </c>
       <c r="I11" s="10" t="inlineStr">
         <is>
@@ -1572,7 +1608,7 @@
         </is>
       </c>
       <c r="J11" s="19" t="n">
-        <v>294878.81</v>
+        <v>55620.91</v>
       </c>
       <c r="K11" s="10" t="inlineStr">
         <is>
@@ -1580,7 +1616,7 @@
         </is>
       </c>
       <c r="L11" s="19" t="n">
-        <v>324584.04</v>
+        <v>55437.02</v>
       </c>
       <c r="M11" s="10" t="inlineStr">
         <is>
@@ -1588,7 +1624,7 @@
         </is>
       </c>
       <c r="N11" s="19" t="n">
-        <v>285670.97</v>
+        <v>56870.56</v>
       </c>
       <c r="O11" s="10" t="inlineStr">
         <is>
@@ -1596,29 +1632,35 @@
         </is>
       </c>
       <c r="P11" s="19" t="n">
-        <v>297512.49</v>
+        <v>52253.08</v>
       </c>
       <c r="Q11" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="R11" s="10" t="inlineStr">
+      <c r="R11" s="19" t="n">
+        <v>52489.84</v>
+      </c>
+      <c r="S11" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T11" s="26" t="n">
+        <v>51413.7</v>
+      </c>
+      <c r="U11" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V11" s="10" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="S11" s="10" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="T11" s="10" t="inlineStr">
-        <is>
-          <t>:</t>
-        </is>
-      </c>
-      <c r="U11" s="10" t="inlineStr">
+      <c r="W11" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -1631,7 +1673,7 @@
         </is>
       </c>
       <c r="B12" s="20" t="n">
-        <v>307946.75</v>
+        <v>54958.77</v>
       </c>
       <c r="C12" s="11" t="inlineStr">
         <is>
@@ -1639,7 +1681,7 @@
         </is>
       </c>
       <c r="D12" s="20" t="n">
-        <v>291716.44</v>
+        <v>55089.61</v>
       </c>
       <c r="E12" s="11" t="inlineStr">
         <is>
@@ -1647,7 +1689,7 @@
         </is>
       </c>
       <c r="F12" s="20" t="n">
-        <v>280101.04</v>
+        <v>54472.74</v>
       </c>
       <c r="G12" s="11" t="inlineStr">
         <is>
@@ -1655,7 +1697,7 @@
         </is>
       </c>
       <c r="H12" s="20" t="n">
-        <v>287259.62</v>
+        <v>54092.53</v>
       </c>
       <c r="I12" s="11" t="inlineStr">
         <is>
@@ -1663,7 +1705,7 @@
         </is>
       </c>
       <c r="J12" s="20" t="n">
-        <v>274038.99</v>
+        <v>52439.91</v>
       </c>
       <c r="K12" s="11" t="inlineStr">
         <is>
@@ -1671,15 +1713,15 @@
         </is>
       </c>
       <c r="L12" s="20" t="n">
-        <v>299364.18</v>
+        <v>52331.22</v>
       </c>
       <c r="M12" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="N12" s="20" t="n">
-        <v>285670.97</v>
+      <c r="N12" s="30" t="n">
+        <v>53659.7</v>
       </c>
       <c r="O12" s="11" t="inlineStr">
         <is>
@@ -1687,29 +1729,35 @@
         </is>
       </c>
       <c r="P12" s="20" t="n">
-        <v>297512.49</v>
+        <v>52253.08</v>
       </c>
       <c r="Q12" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="R12" s="11" t="inlineStr">
+      <c r="R12" s="20" t="n">
+        <v>52489.84</v>
+      </c>
+      <c r="S12" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T12" s="30" t="n">
+        <v>51413.7</v>
+      </c>
+      <c r="U12" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V12" s="11" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="S12" s="11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="T12" s="11" t="inlineStr">
-        <is>
-          <t>:</t>
-        </is>
-      </c>
-      <c r="U12" s="11" t="inlineStr">
+      <c r="W12" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -1721,16 +1769,18 @@
           <t>European Union - 28 countries (2013-2020)</t>
         </is>
       </c>
-      <c r="B13" s="19" t="n">
-        <v>332329.17</v>
+      <c r="B13" s="26" t="n">
+        <v>57993.4</v>
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="D13" s="19" t="n">
-        <v>316307.63</v>
+      <c r="D13" s="10" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
       </c>
       <c r="E13" s="10" t="inlineStr">
         <is>
@@ -1738,7 +1788,7 @@
         </is>
       </c>
       <c r="F13" s="19" t="n">
-        <v>301811.62</v>
+        <v>57571.74</v>
       </c>
       <c r="G13" s="10" t="inlineStr">
         <is>
@@ -1746,7 +1796,7 @@
         </is>
       </c>
       <c r="H13" s="19" t="n">
-        <v>309993.16</v>
+        <v>57220.53</v>
       </c>
       <c r="I13" s="10" t="inlineStr">
         <is>
@@ -1754,7 +1804,7 @@
         </is>
       </c>
       <c r="J13" s="19" t="n">
-        <v>294878.81</v>
+        <v>55620.91</v>
       </c>
       <c r="K13" s="10" t="inlineStr">
         <is>
@@ -1762,49 +1812,57 @@
         </is>
       </c>
       <c r="L13" s="19" t="n">
-        <v>324584.04</v>
+        <v>55437.02</v>
       </c>
       <c r="M13" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="N13" s="10" t="inlineStr">
+      <c r="N13" s="19" t="n">
+        <v>56870.56</v>
+      </c>
+      <c r="O13" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P13" s="10" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="O13" s="10" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P13" s="10" t="inlineStr">
+      <c r="Q13" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="R13" s="10" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="Q13" s="10" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="R13" s="10" t="inlineStr">
+      <c r="S13" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T13" s="10" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="S13" s="10" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="T13" s="10" t="inlineStr">
+      <c r="U13" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V13" s="10" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="U13" s="10" t="inlineStr">
+      <c r="W13" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -1816,8 +1874,8 @@
           <t>Belgium</t>
         </is>
       </c>
-      <c r="B14" s="20" t="n">
-        <v>3054.92</v>
+      <c r="B14" s="30" t="n">
+        <v>337.9</v>
       </c>
       <c r="C14" s="11" t="inlineStr">
         <is>
@@ -1825,7 +1883,7 @@
         </is>
       </c>
       <c r="D14" s="20" t="n">
-        <v>3133.68</v>
+        <v>333.58</v>
       </c>
       <c r="E14" s="11" t="inlineStr">
         <is>
@@ -1833,7 +1891,7 @@
         </is>
       </c>
       <c r="F14" s="20" t="n">
-        <v>2228.79</v>
+        <v>341.64</v>
       </c>
       <c r="G14" s="11" t="inlineStr">
         <is>
@@ -1841,7 +1899,7 @@
         </is>
       </c>
       <c r="H14" s="20" t="n">
-        <v>2642.25</v>
+        <v>337.01</v>
       </c>
       <c r="I14" s="11" t="inlineStr">
         <is>
@@ -1849,7 +1907,7 @@
         </is>
       </c>
       <c r="J14" s="20" t="n">
-        <v>2431.04</v>
+        <v>305.44</v>
       </c>
       <c r="K14" s="11" t="inlineStr">
         <is>
@@ -1857,15 +1915,15 @@
         </is>
       </c>
       <c r="L14" s="20" t="n">
-        <v>2816.04</v>
+        <v>304.52</v>
       </c>
       <c r="M14" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="N14" s="30" t="n">
-        <v>2565.7</v>
+      <c r="N14" s="20" t="n">
+        <v>313.11</v>
       </c>
       <c r="O14" s="11" t="inlineStr">
         <is>
@@ -1873,27 +1931,35 @@
         </is>
       </c>
       <c r="P14" s="20" t="n">
-        <v>2452.66</v>
+        <v>304.34</v>
       </c>
       <c r="Q14" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="R14" s="20" t="n">
-        <v>2753.47</v>
+      <c r="R14" s="30" t="n">
+        <v>310.2</v>
       </c>
       <c r="S14" s="11" t="inlineStr">
         <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T14" s="20" t="n">
+        <v>323.07</v>
+      </c>
+      <c r="U14" s="11" t="inlineStr">
+        <is>
           <t>p</t>
         </is>
       </c>
-      <c r="T14" s="11" t="inlineStr">
+      <c r="V14" s="11" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="U14" s="11" t="inlineStr">
+      <c r="W14" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -1906,15 +1972,15 @@
         </is>
       </c>
       <c r="B15" s="19" t="n">
-        <v>9674.49</v>
+        <v>2006.99</v>
       </c>
       <c r="C15" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="D15" s="19" t="n">
-        <v>8728.97</v>
+      <c r="D15" s="26" t="n">
+        <v>1960.7</v>
       </c>
       <c r="E15" s="10" t="inlineStr">
         <is>
@@ -1922,7 +1988,7 @@
         </is>
       </c>
       <c r="F15" s="19" t="n">
-        <v>8945.12</v>
+        <v>1835.77</v>
       </c>
       <c r="G15" s="10" t="inlineStr">
         <is>
@@ -1930,7 +1996,7 @@
         </is>
       </c>
       <c r="H15" s="19" t="n">
-        <v>9737.28</v>
+        <v>1816.64</v>
       </c>
       <c r="I15" s="10" t="inlineStr">
         <is>
@@ -1938,7 +2004,7 @@
         </is>
       </c>
       <c r="J15" s="19" t="n">
-        <v>10110.55</v>
+        <v>1729.27</v>
       </c>
       <c r="K15" s="10" t="inlineStr">
         <is>
@@ -1946,7 +2012,7 @@
         </is>
       </c>
       <c r="L15" s="19" t="n">
-        <v>11131.81</v>
+        <v>1817.78</v>
       </c>
       <c r="M15" s="10" t="inlineStr">
         <is>
@@ -1954,7 +2020,7 @@
         </is>
       </c>
       <c r="N15" s="19" t="n">
-        <v>8599.06</v>
+        <v>1927.57</v>
       </c>
       <c r="O15" s="10" t="inlineStr">
         <is>
@@ -1962,27 +2028,35 @@
         </is>
       </c>
       <c r="P15" s="19" t="n">
-        <v>11639.98</v>
+        <v>1966.04</v>
       </c>
       <c r="Q15" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="R15" s="26" t="n">
-        <v>9790.0</v>
+      <c r="R15" s="19" t="n">
+        <v>1956.33</v>
       </c>
       <c r="S15" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="T15" s="10" t="inlineStr">
+      <c r="T15" s="26" t="n">
+        <v>1897.7</v>
+      </c>
+      <c r="U15" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V15" s="10" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="U15" s="10" t="inlineStr">
+      <c r="W15" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -1994,8 +2068,8 @@
           <t>Czechia</t>
         </is>
       </c>
-      <c r="B16" s="30" t="n">
-        <v>8779.3</v>
+      <c r="B16" s="20" t="n">
+        <v>1413.14</v>
       </c>
       <c r="C16" s="11" t="inlineStr">
         <is>
@@ -2003,7 +2077,7 @@
         </is>
       </c>
       <c r="D16" s="20" t="n">
-        <v>8183.51</v>
+        <v>1409.61</v>
       </c>
       <c r="E16" s="11" t="inlineStr">
         <is>
@@ -2011,7 +2085,7 @@
         </is>
       </c>
       <c r="F16" s="20" t="n">
-        <v>8596.41</v>
+        <v>1389.83</v>
       </c>
       <c r="G16" s="11" t="inlineStr">
         <is>
@@ -2019,7 +2093,7 @@
         </is>
       </c>
       <c r="H16" s="20" t="n">
-        <v>7456.78</v>
+        <v>1359.01</v>
       </c>
       <c r="I16" s="11" t="inlineStr">
         <is>
@@ -2027,7 +2101,7 @@
         </is>
       </c>
       <c r="J16" s="20" t="n">
-        <v>6970.92</v>
+        <v>1354.68</v>
       </c>
       <c r="K16" s="11" t="inlineStr">
         <is>
@@ -2035,7 +2109,7 @@
         </is>
       </c>
       <c r="L16" s="20" t="n">
-        <v>7646.15</v>
+        <v>1338.78</v>
       </c>
       <c r="M16" s="11" t="inlineStr">
         <is>
@@ -2043,7 +2117,7 @@
         </is>
       </c>
       <c r="N16" s="20" t="n">
-        <v>8126.66</v>
+        <v>1352.53</v>
       </c>
       <c r="O16" s="11" t="inlineStr">
         <is>
@@ -2051,7 +2125,7 @@
         </is>
       </c>
       <c r="P16" s="20" t="n">
-        <v>8227.11</v>
+        <v>1344.88</v>
       </c>
       <c r="Q16" s="11" t="inlineStr">
         <is>
@@ -2059,19 +2133,25 @@
         </is>
       </c>
       <c r="R16" s="20" t="n">
-        <v>8218.42</v>
+        <v>1345.84</v>
       </c>
       <c r="S16" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="T16" s="11" t="inlineStr">
-        <is>
-          <t>:</t>
-        </is>
+      <c r="T16" s="20" t="n">
+        <v>1386.01</v>
       </c>
       <c r="U16" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V16" s="20" t="n">
+        <v>1326.54</v>
+      </c>
+      <c r="W16" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -2083,72 +2163,72 @@
           <t>Denmark</t>
         </is>
       </c>
-      <c r="B17" s="19" t="n">
-        <v>9650.86</v>
+      <c r="B17" s="26" t="n">
+        <v>1426.1</v>
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="D17" s="19" t="n">
-        <v>9907.84</v>
+      <c r="D17" s="26" t="n">
+        <v>1442.7</v>
       </c>
       <c r="E17" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="F17" s="19" t="n">
-        <v>9024.03</v>
+      <c r="F17" s="26" t="n">
+        <v>1454.4</v>
       </c>
       <c r="G17" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="H17" s="19" t="n">
-        <v>9882.96</v>
+      <c r="H17" s="26" t="n">
+        <v>1464.8</v>
       </c>
       <c r="I17" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J17" s="19" t="n">
-        <v>6923.84</v>
+      <c r="J17" s="26" t="n">
+        <v>1442.7</v>
       </c>
       <c r="K17" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="L17" s="19" t="n">
-        <v>9517.92</v>
+      <c r="L17" s="26" t="n">
+        <v>1416.3</v>
       </c>
       <c r="M17" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="N17" s="19" t="n">
-        <v>9467.62</v>
+      <c r="N17" s="26" t="n">
+        <v>1373.7</v>
       </c>
       <c r="O17" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="P17" s="19" t="n">
-        <v>8640.05</v>
+      <c r="P17" s="26" t="n">
+        <v>1367.0</v>
       </c>
       <c r="Q17" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="R17" s="19" t="n">
-        <v>9464.18</v>
+      <c r="R17" s="26" t="n">
+        <v>1359.7</v>
       </c>
       <c r="S17" s="10" t="inlineStr">
         <is>
@@ -2156,9 +2236,17 @@
         </is>
       </c>
       <c r="T17" s="19" t="n">
-        <v>6641.26</v>
+        <v>1306.95</v>
       </c>
       <c r="U17" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V17" s="19" t="n">
+        <v>1229.51</v>
+      </c>
+      <c r="W17" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -2171,7 +2259,7 @@
         </is>
       </c>
       <c r="B18" s="30" t="n">
-        <v>52048.2</v>
+        <v>6533.7</v>
       </c>
       <c r="C18" s="11" t="inlineStr">
         <is>
@@ -2179,7 +2267,7 @@
         </is>
       </c>
       <c r="D18" s="30" t="n">
-        <v>48917.7</v>
+        <v>6468.6</v>
       </c>
       <c r="E18" s="11" t="inlineStr">
         <is>
@@ -2187,7 +2275,7 @@
         </is>
       </c>
       <c r="F18" s="30" t="n">
-        <v>45401.0</v>
+        <v>6529.2</v>
       </c>
       <c r="G18" s="11" t="inlineStr">
         <is>
@@ -2195,7 +2283,7 @@
         </is>
       </c>
       <c r="H18" s="30" t="n">
-        <v>45593.2</v>
+        <v>6325.0</v>
       </c>
       <c r="I18" s="11" t="inlineStr">
         <is>
@@ -2203,7 +2291,7 @@
         </is>
       </c>
       <c r="J18" s="30" t="n">
-        <v>37974.8</v>
+        <v>6276.2</v>
       </c>
       <c r="K18" s="11" t="inlineStr">
         <is>
@@ -2211,7 +2299,7 @@
         </is>
       </c>
       <c r="L18" s="30" t="n">
-        <v>44329.3</v>
+        <v>6148.9</v>
       </c>
       <c r="M18" s="11" t="inlineStr">
         <is>
@@ -2219,7 +2307,7 @@
         </is>
       </c>
       <c r="N18" s="30" t="n">
-        <v>43301.2</v>
+        <v>6380.0</v>
       </c>
       <c r="O18" s="11" t="inlineStr">
         <is>
@@ -2227,7 +2315,7 @@
         </is>
       </c>
       <c r="P18" s="30" t="n">
-        <v>42397.6</v>
+        <v>6074.9</v>
       </c>
       <c r="Q18" s="11" t="inlineStr">
         <is>
@@ -2235,19 +2323,25 @@
         </is>
       </c>
       <c r="R18" s="30" t="n">
-        <v>43520.8</v>
+        <v>6063.5</v>
       </c>
       <c r="S18" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="T18" s="11" t="inlineStr">
-        <is>
-          <t>:</t>
-        </is>
+      <c r="T18" s="30" t="n">
+        <v>6112.5</v>
       </c>
       <c r="U18" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V18" s="30" t="n">
+        <v>6091.3</v>
+      </c>
+      <c r="W18" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -2260,7 +2354,7 @@
         </is>
       </c>
       <c r="B19" s="26" t="n">
-        <v>1221.6</v>
+        <v>311.1</v>
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
@@ -2268,7 +2362,7 @@
         </is>
       </c>
       <c r="D19" s="26" t="n">
-        <v>1535.3</v>
+        <v>332.9</v>
       </c>
       <c r="E19" s="10" t="inlineStr">
         <is>
@@ -2276,7 +2370,7 @@
         </is>
       </c>
       <c r="F19" s="26" t="n">
-        <v>934.1</v>
+        <v>350.4</v>
       </c>
       <c r="G19" s="10" t="inlineStr">
         <is>
@@ -2284,7 +2378,7 @@
         </is>
       </c>
       <c r="H19" s="26" t="n">
-        <v>1311.9</v>
+        <v>351.4</v>
       </c>
       <c r="I19" s="10" t="inlineStr">
         <is>
@@ -2292,7 +2386,7 @@
         </is>
       </c>
       <c r="J19" s="19" t="n">
-        <v>919.83</v>
+        <v>330.68</v>
       </c>
       <c r="K19" s="10" t="inlineStr">
         <is>
@@ -2300,7 +2394,7 @@
         </is>
       </c>
       <c r="L19" s="19" t="n">
-        <v>1624.58</v>
+        <v>350.43</v>
       </c>
       <c r="M19" s="10" t="inlineStr">
         <is>
@@ -2308,7 +2402,7 @@
         </is>
       </c>
       <c r="N19" s="19" t="n">
-        <v>1632.79</v>
+        <v>364.36</v>
       </c>
       <c r="O19" s="10" t="inlineStr">
         <is>
@@ -2316,7 +2410,7 @@
         </is>
       </c>
       <c r="P19" s="19" t="n">
-        <v>1285.75</v>
+        <v>370.12</v>
       </c>
       <c r="Q19" s="10" t="inlineStr">
         <is>
@@ -2324,19 +2418,25 @@
         </is>
       </c>
       <c r="R19" s="19" t="n">
-        <v>1528.55</v>
+        <v>367.12</v>
       </c>
       <c r="S19" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="T19" s="10" t="inlineStr">
-        <is>
-          <t>:</t>
-        </is>
+      <c r="T19" s="19" t="n">
+        <v>361.82</v>
       </c>
       <c r="U19" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V19" s="19" t="n">
+        <v>351.23</v>
+      </c>
+      <c r="W19" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -2348,8 +2448,8 @@
           <t>Ireland</t>
         </is>
       </c>
-      <c r="B20" s="20" t="n">
-        <v>2491.52</v>
+      <c r="B20" s="30" t="n">
+        <v>306.7</v>
       </c>
       <c r="C20" s="11" t="inlineStr">
         <is>
@@ -2357,7 +2457,7 @@
         </is>
       </c>
       <c r="D20" s="20" t="n">
-        <v>2497.93</v>
+        <v>305.89</v>
       </c>
       <c r="E20" s="11" t="inlineStr">
         <is>
@@ -2365,7 +2465,7 @@
         </is>
       </c>
       <c r="F20" s="20" t="n">
-        <v>2184.32</v>
+        <v>291.56</v>
       </c>
       <c r="G20" s="11" t="inlineStr">
         <is>
@@ -2373,7 +2473,7 @@
         </is>
       </c>
       <c r="H20" s="20" t="n">
-        <v>2259.53</v>
+        <v>280.34</v>
       </c>
       <c r="I20" s="11" t="inlineStr">
         <is>
@@ -2381,15 +2481,15 @@
         </is>
       </c>
       <c r="J20" s="20" t="n">
-        <v>1784.91</v>
+        <v>271.68</v>
       </c>
       <c r="K20" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="L20" s="30" t="n">
-        <v>2268.0</v>
+      <c r="L20" s="20" t="n">
+        <v>260.97</v>
       </c>
       <c r="M20" s="11" t="inlineStr">
         <is>
@@ -2397,7 +2497,7 @@
         </is>
       </c>
       <c r="N20" s="20" t="n">
-        <v>1892.63</v>
+        <v>266.66</v>
       </c>
       <c r="O20" s="11" t="inlineStr">
         <is>
@@ -2405,7 +2505,7 @@
         </is>
       </c>
       <c r="P20" s="20" t="n">
-        <v>2363.97</v>
+        <v>265.63</v>
       </c>
       <c r="Q20" s="11" t="inlineStr">
         <is>
@@ -2413,19 +2513,25 @@
         </is>
       </c>
       <c r="R20" s="20" t="n">
-        <v>2453.95</v>
+        <v>274.66</v>
       </c>
       <c r="S20" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="T20" s="11" t="inlineStr">
-        <is>
-          <t>:</t>
-        </is>
+      <c r="T20" s="20" t="n">
+        <v>282.46</v>
       </c>
       <c r="U20" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V20" s="20" t="n">
+        <v>268.91</v>
+      </c>
+      <c r="W20" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -2438,7 +2544,7 @@
         </is>
       </c>
       <c r="B21" s="19" t="n">
-        <v>4565.11</v>
+        <v>1034.84</v>
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
@@ -2446,7 +2552,7 @@
         </is>
       </c>
       <c r="D21" s="19" t="n">
-        <v>3588.78</v>
+        <v>1034.29</v>
       </c>
       <c r="E21" s="10" t="inlineStr">
         <is>
@@ -2454,7 +2560,7 @@
         </is>
       </c>
       <c r="F21" s="19" t="n">
-        <v>3983.13</v>
+        <v>959.01</v>
       </c>
       <c r="G21" s="10" t="inlineStr">
         <is>
@@ -2462,7 +2568,7 @@
         </is>
       </c>
       <c r="H21" s="19" t="n">
-        <v>3015.72</v>
+        <v>987.95</v>
       </c>
       <c r="I21" s="10" t="inlineStr">
         <is>
@@ -2470,7 +2576,7 @@
         </is>
       </c>
       <c r="J21" s="19" t="n">
-        <v>2996.56</v>
+        <v>839.17</v>
       </c>
       <c r="K21" s="10" t="inlineStr">
         <is>
@@ -2478,7 +2584,7 @@
         </is>
       </c>
       <c r="L21" s="19" t="n">
-        <v>2946.78</v>
+        <v>787.98</v>
       </c>
       <c r="M21" s="10" t="inlineStr">
         <is>
@@ -2486,7 +2592,7 @@
         </is>
       </c>
       <c r="N21" s="19" t="n">
-        <v>3108.73</v>
+        <v>728.14</v>
       </c>
       <c r="O21" s="10" t="inlineStr">
         <is>
@@ -2494,15 +2600,15 @@
         </is>
       </c>
       <c r="P21" s="19" t="n">
-        <v>3095.45</v>
+        <v>739.88</v>
       </c>
       <c r="Q21" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="R21" s="26" t="n">
-        <v>2564.0</v>
+      <c r="R21" s="19" t="n">
+        <v>723.81</v>
       </c>
       <c r="S21" s="10" t="inlineStr">
         <is>
@@ -2510,9 +2616,17 @@
         </is>
       </c>
       <c r="T21" s="19" t="n">
-        <v>2544.65</v>
+        <v>675.77</v>
       </c>
       <c r="U21" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V21" s="19" t="n">
+        <v>656.02</v>
+      </c>
+      <c r="W21" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -2525,7 +2639,7 @@
         </is>
       </c>
       <c r="B22" s="20" t="n">
-        <v>20564.24</v>
+        <v>6268.03</v>
       </c>
       <c r="C22" s="11" t="inlineStr">
         <is>
@@ -2533,7 +2647,7 @@
         </is>
       </c>
       <c r="D22" s="20" t="n">
-        <v>20783.82</v>
+        <v>6313.11</v>
       </c>
       <c r="E22" s="11" t="inlineStr">
         <is>
@@ -2541,15 +2655,15 @@
         </is>
       </c>
       <c r="F22" s="20" t="n">
-        <v>24955.45</v>
+        <v>6195.86</v>
       </c>
       <c r="G22" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="H22" s="20" t="n">
-        <v>17188.44</v>
+      <c r="H22" s="30" t="n">
+        <v>6239.8</v>
       </c>
       <c r="I22" s="11" t="inlineStr">
         <is>
@@ -2557,7 +2671,7 @@
         </is>
       </c>
       <c r="J22" s="20" t="n">
-        <v>25358.14</v>
+        <v>6015.23</v>
       </c>
       <c r="K22" s="11" t="inlineStr">
         <is>
@@ -2565,7 +2679,7 @@
         </is>
       </c>
       <c r="L22" s="20" t="n">
-        <v>20598.15</v>
+        <v>6027.61</v>
       </c>
       <c r="M22" s="11" t="inlineStr">
         <is>
@@ -2573,33 +2687,41 @@
         </is>
       </c>
       <c r="N22" s="20" t="n">
-        <v>27329.48</v>
+        <v>5975.71</v>
       </c>
       <c r="O22" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="P22" s="30" t="n">
-        <v>25517.6</v>
+      <c r="P22" s="20" t="n">
+        <v>6069.24</v>
       </c>
       <c r="Q22" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="R22" s="30" t="n">
-        <v>19055.6</v>
+      <c r="R22" s="20" t="n">
+        <v>6034.58</v>
       </c>
       <c r="S22" s="11" t="inlineStr">
         <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T22" s="20" t="n">
+        <v>5804.21</v>
+      </c>
+      <c r="U22" s="11" t="inlineStr">
+        <is>
           <t>p</t>
         </is>
       </c>
-      <c r="T22" s="20" t="n">
-        <v>13226.37</v>
-      </c>
-      <c r="U22" s="11" t="inlineStr">
+      <c r="V22" s="30" t="n">
+        <v>5496.0</v>
+      </c>
+      <c r="W22" s="11" t="inlineStr">
         <is>
           <t>p</t>
         </is>
@@ -2611,8 +2733,8 @@
           <t>France</t>
         </is>
       </c>
-      <c r="B23" s="26" t="n">
-        <v>71588.8</v>
+      <c r="B23" s="19" t="n">
+        <v>9476.27</v>
       </c>
       <c r="C23" s="10" t="inlineStr">
         <is>
@@ -2620,7 +2742,7 @@
         </is>
       </c>
       <c r="D23" s="19" t="n">
-        <v>71870.79</v>
+        <v>9563.41</v>
       </c>
       <c r="E23" s="10" t="inlineStr">
         <is>
@@ -2628,7 +2750,7 @@
         </is>
       </c>
       <c r="F23" s="19" t="n">
-        <v>53560.42</v>
+        <v>9584.58</v>
       </c>
       <c r="G23" s="10" t="inlineStr">
         <is>
@@ -2636,7 +2758,7 @@
         </is>
       </c>
       <c r="H23" s="19" t="n">
-        <v>67728.63</v>
+        <v>9529.98</v>
       </c>
       <c r="I23" s="10" t="inlineStr">
         <is>
@@ -2644,7 +2766,7 @@
         </is>
       </c>
       <c r="J23" s="19" t="n">
-        <v>61840.31</v>
+        <v>9339.87</v>
       </c>
       <c r="K23" s="10" t="inlineStr">
         <is>
@@ -2652,7 +2774,7 @@
         </is>
       </c>
       <c r="L23" s="19" t="n">
-        <v>70379.86</v>
+        <v>9055.31</v>
       </c>
       <c r="M23" s="10" t="inlineStr">
         <is>
@@ -2660,23 +2782,23 @@
         </is>
       </c>
       <c r="N23" s="19" t="n">
-        <v>57086.04</v>
+        <v>9394.03</v>
       </c>
       <c r="O23" s="10" t="inlineStr">
         <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P23" s="19" t="n">
+        <v>8926.69</v>
+      </c>
+      <c r="Q23" s="10" t="inlineStr">
+        <is>
           <t>b</t>
         </is>
       </c>
-      <c r="P23" s="19" t="n">
-        <v>66877.88</v>
-      </c>
-      <c r="Q23" s="10" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
       <c r="R23" s="26" t="n">
-        <v>59673.5</v>
+        <v>9325.7</v>
       </c>
       <c r="S23" s="10" t="inlineStr">
         <is>
@@ -2684,9 +2806,17 @@
         </is>
       </c>
       <c r="T23" s="19" t="n">
-        <v>62633.88</v>
+        <v>8967.43</v>
       </c>
       <c r="U23" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V23" s="19" t="n">
+        <v>8766.69</v>
+      </c>
+      <c r="W23" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -2698,8 +2828,8 @@
           <t>Croatia</t>
         </is>
       </c>
-      <c r="B24" s="30" t="n">
-        <v>2967.6</v>
+      <c r="B24" s="20" t="n">
+        <v>570.04</v>
       </c>
       <c r="C24" s="11" t="inlineStr">
         <is>
@@ -2707,7 +2837,7 @@
         </is>
       </c>
       <c r="D24" s="20" t="n">
-        <v>2773.95</v>
+        <v>478.52</v>
       </c>
       <c r="E24" s="11" t="inlineStr">
         <is>
@@ -2715,7 +2845,7 @@
         </is>
       </c>
       <c r="F24" s="20" t="n">
-        <v>3554.43</v>
+        <v>475.64</v>
       </c>
       <c r="G24" s="11" t="inlineStr">
         <is>
@@ -2723,7 +2853,7 @@
         </is>
       </c>
       <c r="H24" s="20" t="n">
-        <v>2678.79</v>
+        <v>528.47</v>
       </c>
       <c r="I24" s="11" t="inlineStr">
         <is>
@@ -2731,15 +2861,15 @@
         </is>
       </c>
       <c r="J24" s="20" t="n">
-        <v>3268.48</v>
+        <v>461.48</v>
       </c>
       <c r="K24" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="L24" s="20" t="n">
-        <v>3540.05</v>
+      <c r="L24" s="30" t="n">
+        <v>459.7</v>
       </c>
       <c r="M24" s="11" t="inlineStr">
         <is>
@@ -2747,7 +2877,7 @@
         </is>
       </c>
       <c r="N24" s="20" t="n">
-        <v>3774.57</v>
+        <v>490.88</v>
       </c>
       <c r="O24" s="11" t="inlineStr">
         <is>
@@ -2755,7 +2885,7 @@
         </is>
       </c>
       <c r="P24" s="20" t="n">
-        <v>3671.23</v>
+        <v>535.76</v>
       </c>
       <c r="Q24" s="11" t="inlineStr">
         <is>
@@ -2763,19 +2893,27 @@
         </is>
       </c>
       <c r="R24" s="20" t="n">
-        <v>3080.51</v>
+        <v>519.78</v>
       </c>
       <c r="S24" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="T24" s="11" t="inlineStr">
+      <c r="T24" s="30" t="n">
+        <v>525.6</v>
+      </c>
+      <c r="U24" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V24" s="11" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="U24" s="11" t="inlineStr">
+      <c r="W24" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -2788,7 +2926,7 @@
         </is>
       </c>
       <c r="B25" s="19" t="n">
-        <v>19769.47</v>
+        <v>3459.87</v>
       </c>
       <c r="C25" s="10" t="inlineStr">
         <is>
@@ -2796,15 +2934,15 @@
         </is>
       </c>
       <c r="D25" s="19" t="n">
-        <v>17462.24</v>
+        <v>3392.95</v>
       </c>
       <c r="E25" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="F25" s="26" t="n">
-        <v>18363.1</v>
+      <c r="F25" s="19" t="n">
+        <v>3191.48</v>
       </c>
       <c r="G25" s="10" t="inlineStr">
         <is>
@@ -2812,7 +2950,7 @@
         </is>
       </c>
       <c r="H25" s="19" t="n">
-        <v>16554.95</v>
+        <v>3256.99</v>
       </c>
       <c r="I25" s="10" t="inlineStr">
         <is>
@@ -2820,23 +2958,23 @@
         </is>
       </c>
       <c r="J25" s="19" t="n">
-        <v>16615.46</v>
+        <v>3140.58</v>
       </c>
       <c r="K25" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="L25" s="26" t="n">
-        <v>16433.5</v>
+      <c r="L25" s="19" t="n">
+        <v>3092.69</v>
       </c>
       <c r="M25" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="N25" s="26" t="n">
-        <v>17022.9</v>
+      <c r="N25" s="19" t="n">
+        <v>3066.52</v>
       </c>
       <c r="O25" s="10" t="inlineStr">
         <is>
@@ -2844,29 +2982,33 @@
         </is>
       </c>
       <c r="P25" s="19" t="n">
-        <v>16632.66</v>
+        <v>3011.73</v>
       </c>
       <c r="Q25" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="R25" s="10" t="inlineStr">
-        <is>
-          <t>:</t>
-        </is>
+      <c r="R25" s="19" t="n">
+        <v>2978.39</v>
       </c>
       <c r="S25" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="T25" s="10" t="inlineStr">
-        <is>
-          <t>:</t>
-        </is>
+      <c r="T25" s="19" t="n">
+        <v>3014.94</v>
       </c>
       <c r="U25" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V25" s="19" t="n">
+        <v>3073.63</v>
+      </c>
+      <c r="W25" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -2879,15 +3021,15 @@
         </is>
       </c>
       <c r="B26" s="20" t="n">
-        <v>7.36</v>
+        <v>30.76</v>
       </c>
       <c r="C26" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="D26" s="20" t="n">
-        <v>88.13</v>
+      <c r="D26" s="30" t="n">
+        <v>25.3</v>
       </c>
       <c r="E26" s="11" t="inlineStr">
         <is>
@@ -2895,15 +3037,15 @@
         </is>
       </c>
       <c r="F26" s="20" t="n">
-        <v>10.42</v>
+        <v>32.85</v>
       </c>
       <c r="G26" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="H26" s="20" t="n">
-        <v>36.45</v>
+      <c r="H26" s="30" t="n">
+        <v>23.8</v>
       </c>
       <c r="I26" s="11" t="inlineStr">
         <is>
@@ -2911,7 +3053,7 @@
         </is>
       </c>
       <c r="J26" s="20" t="n">
-        <v>24.71</v>
+        <v>20.22</v>
       </c>
       <c r="K26" s="11" t="inlineStr">
         <is>
@@ -2919,7 +3061,7 @@
         </is>
       </c>
       <c r="L26" s="20" t="n">
-        <v>59.03</v>
+        <v>24.01</v>
       </c>
       <c r="M26" s="11" t="inlineStr">
         <is>
@@ -2927,7 +3069,7 @@
         </is>
       </c>
       <c r="N26" s="20" t="n">
-        <v>60.96</v>
+        <v>23.07</v>
       </c>
       <c r="O26" s="11" t="inlineStr">
         <is>
@@ -2935,25 +3077,33 @@
         </is>
       </c>
       <c r="P26" s="20" t="n">
-        <v>51.22</v>
+        <v>26.52</v>
       </c>
       <c r="Q26" s="11" t="inlineStr">
         <is>
+          <t/>
+        </is>
+      </c>
+      <c r="R26" s="20" t="n">
+        <v>26.45</v>
+      </c>
+      <c r="S26" s="11" t="inlineStr">
+        <is>
           <t>p</t>
         </is>
       </c>
-      <c r="R26" s="20" t="n">
-        <v>59.58</v>
-      </c>
-      <c r="S26" s="11" t="inlineStr">
+      <c r="T26" s="20" t="n">
+        <v>24.58</v>
+      </c>
+      <c r="U26" s="11" t="inlineStr">
         <is>
           <t>e</t>
         </is>
       </c>
-      <c r="T26" s="30" t="n">
-        <v>46.3</v>
-      </c>
-      <c r="U26" s="11" t="inlineStr">
+      <c r="V26" s="30" t="n">
+        <v>23.4</v>
+      </c>
+      <c r="W26" s="11" t="inlineStr">
         <is>
           <t>e</t>
         </is>
@@ -2966,7 +3116,7 @@
         </is>
       </c>
       <c r="B27" s="26" t="n">
-        <v>2227.2</v>
+        <v>577.6</v>
       </c>
       <c r="C27" s="10" t="inlineStr">
         <is>
@@ -2974,7 +3124,7 @@
         </is>
       </c>
       <c r="D27" s="26" t="n">
-        <v>3021.5</v>
+        <v>638.8</v>
       </c>
       <c r="E27" s="10" t="inlineStr">
         <is>
@@ -2982,7 +3132,7 @@
         </is>
       </c>
       <c r="F27" s="26" t="n">
-        <v>2703.2</v>
+        <v>669.5</v>
       </c>
       <c r="G27" s="10" t="inlineStr">
         <is>
@@ -2990,7 +3140,7 @@
         </is>
       </c>
       <c r="H27" s="26" t="n">
-        <v>2692.5</v>
+        <v>706.1</v>
       </c>
       <c r="I27" s="10" t="inlineStr">
         <is>
@@ -2998,7 +3148,7 @@
         </is>
       </c>
       <c r="J27" s="26" t="n">
-        <v>2057.3</v>
+        <v>633.4</v>
       </c>
       <c r="K27" s="10" t="inlineStr">
         <is>
@@ -3006,7 +3156,7 @@
         </is>
       </c>
       <c r="L27" s="26" t="n">
-        <v>3163.2</v>
+        <v>679.8</v>
       </c>
       <c r="M27" s="10" t="inlineStr">
         <is>
@@ -3014,7 +3164,7 @@
         </is>
       </c>
       <c r="N27" s="26" t="n">
-        <v>3497.1</v>
+        <v>733.9</v>
       </c>
       <c r="O27" s="10" t="inlineStr">
         <is>
@@ -3022,7 +3172,7 @@
         </is>
       </c>
       <c r="P27" s="26" t="n">
-        <v>2994.6</v>
+        <v>750.0</v>
       </c>
       <c r="Q27" s="10" t="inlineStr">
         <is>
@@ -3030,19 +3180,27 @@
         </is>
       </c>
       <c r="R27" s="26" t="n">
-        <v>3243.7</v>
+        <v>767.8</v>
       </c>
       <c r="S27" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="T27" s="10" t="inlineStr">
+      <c r="T27" s="26" t="n">
+        <v>774.9</v>
+      </c>
+      <c r="U27" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V27" s="10" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="U27" s="10" t="inlineStr">
+      <c r="W27" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -3055,15 +3213,15 @@
         </is>
       </c>
       <c r="B28" s="30" t="n">
-        <v>5123.2</v>
+        <v>1213.4</v>
       </c>
       <c r="C28" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="D28" s="20" t="n">
-        <v>6085.05</v>
+      <c r="D28" s="30" t="n">
+        <v>1288.8</v>
       </c>
       <c r="E28" s="11" t="inlineStr">
         <is>
@@ -3071,23 +3229,23 @@
         </is>
       </c>
       <c r="F28" s="20" t="n">
-        <v>5120.82</v>
+        <v>1329.12</v>
       </c>
       <c r="G28" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="H28" s="20" t="n">
-        <v>5074.19</v>
+      <c r="H28" s="30" t="n">
+        <v>1326.7</v>
       </c>
       <c r="I28" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J28" s="30" t="n">
-        <v>3999.5</v>
+      <c r="J28" s="20" t="n">
+        <v>1199.51</v>
       </c>
       <c r="K28" s="11" t="inlineStr">
         <is>
@@ -3095,7 +3253,7 @@
         </is>
       </c>
       <c r="L28" s="20" t="n">
-        <v>5207.89</v>
+        <v>1257.23</v>
       </c>
       <c r="M28" s="11" t="inlineStr">
         <is>
@@ -3103,7 +3261,7 @@
         </is>
       </c>
       <c r="N28" s="20" t="n">
-        <v>6544.69</v>
+        <v>1349.57</v>
       </c>
       <c r="O28" s="11" t="inlineStr">
         <is>
@@ -3111,7 +3269,7 @@
         </is>
       </c>
       <c r="P28" s="20" t="n">
-        <v>5340.82</v>
+        <v>1382.43</v>
       </c>
       <c r="Q28" s="11" t="inlineStr">
         <is>
@@ -3119,17 +3277,25 @@
         </is>
       </c>
       <c r="R28" s="20" t="n">
-        <v>5623.66</v>
+        <v>1356.51</v>
       </c>
       <c r="S28" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="T28" s="30" t="n">
-        <v>5394.2</v>
+      <c r="T28" s="20" t="n">
+        <v>1335.72</v>
       </c>
       <c r="U28" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V28" s="30" t="n">
+        <v>1366.6</v>
+      </c>
+      <c r="W28" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -3142,15 +3308,15 @@
         </is>
       </c>
       <c r="B29" s="19" t="n">
-        <v>167.07</v>
+        <v>29.07</v>
       </c>
       <c r="C29" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="D29" s="19" t="n">
-        <v>178.57</v>
+      <c r="D29" s="26" t="n">
+        <v>28.4</v>
       </c>
       <c r="E29" s="10" t="inlineStr">
         <is>
@@ -3158,7 +3324,7 @@
         </is>
       </c>
       <c r="F29" s="19" t="n">
-        <v>139.43</v>
+        <v>29.29</v>
       </c>
       <c r="G29" s="10" t="inlineStr">
         <is>
@@ -3166,7 +3332,7 @@
         </is>
       </c>
       <c r="H29" s="19" t="n">
-        <v>149.81</v>
+        <v>27.86</v>
       </c>
       <c r="I29" s="10" t="inlineStr">
         <is>
@@ -3174,7 +3340,7 @@
         </is>
       </c>
       <c r="J29" s="19" t="n">
-        <v>157.65</v>
+        <v>27.96</v>
       </c>
       <c r="K29" s="10" t="inlineStr">
         <is>
@@ -3182,7 +3348,7 @@
         </is>
       </c>
       <c r="L29" s="19" t="n">
-        <v>163.56</v>
+        <v>26.31</v>
       </c>
       <c r="M29" s="10" t="inlineStr">
         <is>
@@ -3190,7 +3356,7 @@
         </is>
       </c>
       <c r="N29" s="19" t="n">
-        <v>146.17</v>
+        <v>27.39</v>
       </c>
       <c r="O29" s="10" t="inlineStr">
         <is>
@@ -3198,27 +3364,33 @@
         </is>
       </c>
       <c r="P29" s="19" t="n">
-        <v>147.17</v>
+        <v>25.48</v>
       </c>
       <c r="Q29" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="R29" s="19" t="n">
-        <v>170.66</v>
+      <c r="R29" s="26" t="n">
+        <v>26.3</v>
       </c>
       <c r="S29" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="T29" s="10" t="inlineStr">
-        <is>
-          <t>:</t>
-        </is>
+      <c r="T29" s="19" t="n">
+        <v>27.74</v>
       </c>
       <c r="U29" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V29" s="19" t="n">
+        <v>26.72</v>
+      </c>
+      <c r="W29" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -3231,7 +3403,7 @@
         </is>
       </c>
       <c r="B30" s="20" t="n">
-        <v>16559.29</v>
+        <v>2819.94</v>
       </c>
       <c r="C30" s="11" t="inlineStr">
         <is>
@@ -3239,15 +3411,15 @@
         </is>
       </c>
       <c r="D30" s="20" t="n">
-        <v>14107.34</v>
+        <v>2817.27</v>
       </c>
       <c r="E30" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="F30" s="20" t="n">
-        <v>16594.35</v>
+      <c r="F30" s="30" t="n">
+        <v>2697.7</v>
       </c>
       <c r="G30" s="11" t="inlineStr">
         <is>
@@ -3255,7 +3427,7 @@
         </is>
       </c>
       <c r="H30" s="20" t="n">
-        <v>13979.39</v>
+        <v>2566.76</v>
       </c>
       <c r="I30" s="11" t="inlineStr">
         <is>
@@ -3263,7 +3435,7 @@
         </is>
       </c>
       <c r="J30" s="20" t="n">
-        <v>14890.26</v>
+        <v>2403.18</v>
       </c>
       <c r="K30" s="11" t="inlineStr">
         <is>
@@ -3271,7 +3443,7 @@
         </is>
       </c>
       <c r="L30" s="20" t="n">
-        <v>15643.37</v>
+        <v>2367.96</v>
       </c>
       <c r="M30" s="11" t="inlineStr">
         <is>
@@ -3279,7 +3451,7 @@
         </is>
       </c>
       <c r="N30" s="20" t="n">
-        <v>15561.08</v>
+        <v>2458.45</v>
       </c>
       <c r="O30" s="11" t="inlineStr">
         <is>
@@ -3287,7 +3459,7 @@
         </is>
       </c>
       <c r="P30" s="20" t="n">
-        <v>13969.54</v>
+        <v>2337.65</v>
       </c>
       <c r="Q30" s="11" t="inlineStr">
         <is>
@@ -3295,7 +3467,7 @@
         </is>
       </c>
       <c r="R30" s="20" t="n">
-        <v>8872.15</v>
+        <v>2361.64</v>
       </c>
       <c r="S30" s="11" t="inlineStr">
         <is>
@@ -3303,9 +3475,17 @@
         </is>
       </c>
       <c r="T30" s="20" t="n">
-        <v>14763.65</v>
+        <v>2208.81</v>
       </c>
       <c r="U30" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V30" s="20" t="n">
+        <v>2412.15</v>
+      </c>
+      <c r="W30" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -3397,6 +3577,14 @@
           <t/>
         </is>
       </c>
+      <c r="V31" s="26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W31" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="8" t="inlineStr">
@@ -3404,16 +3592,16 @@
           <t>Netherlands</t>
         </is>
       </c>
-      <c r="B32" s="20" t="n">
-        <v>1668.99</v>
+      <c r="B32" s="30" t="n">
+        <v>210.0</v>
       </c>
       <c r="C32" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="D32" s="20" t="n">
-        <v>1629.08</v>
+      <c r="D32" s="30" t="n">
+        <v>192.0</v>
       </c>
       <c r="E32" s="11" t="inlineStr">
         <is>
@@ -3421,7 +3609,7 @@
         </is>
       </c>
       <c r="F32" s="30" t="n">
-        <v>1344.3</v>
+        <v>195.6</v>
       </c>
       <c r="G32" s="11" t="inlineStr">
         <is>
@@ -3429,7 +3617,7 @@
         </is>
       </c>
       <c r="H32" s="20" t="n">
-        <v>1370.62</v>
+        <v>179.16</v>
       </c>
       <c r="I32" s="11" t="inlineStr">
         <is>
@@ -3437,7 +3625,7 @@
         </is>
       </c>
       <c r="J32" s="20" t="n">
-        <v>1315.25</v>
+        <v>162.88</v>
       </c>
       <c r="K32" s="11" t="inlineStr">
         <is>
@@ -3445,7 +3633,7 @@
         </is>
       </c>
       <c r="L32" s="20" t="n">
-        <v>1541.91</v>
+        <v>166.38</v>
       </c>
       <c r="M32" s="11" t="inlineStr">
         <is>
@@ -3453,7 +3641,7 @@
         </is>
       </c>
       <c r="N32" s="20" t="n">
-        <v>1364.38</v>
+        <v>178.16</v>
       </c>
       <c r="O32" s="11" t="inlineStr">
         <is>
@@ -3461,7 +3649,7 @@
         </is>
       </c>
       <c r="P32" s="20" t="n">
-        <v>1336.32</v>
+        <v>172.27</v>
       </c>
       <c r="Q32" s="11" t="inlineStr">
         <is>
@@ -3469,19 +3657,27 @@
         </is>
       </c>
       <c r="R32" s="20" t="n">
-        <v>1647.11</v>
+        <v>169.73</v>
       </c>
       <c r="S32" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="T32" s="11" t="inlineStr">
+      <c r="T32" s="20" t="n">
+        <v>185.41</v>
+      </c>
+      <c r="U32" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V32" s="11" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="U32" s="11" t="inlineStr">
+      <c r="W32" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -3493,24 +3689,24 @@
           <t>Austria</t>
         </is>
       </c>
-      <c r="B33" s="19" t="n">
-        <v>5710.27</v>
+      <c r="B33" s="26" t="n">
+        <v>784.0</v>
       </c>
       <c r="C33" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="D33" s="26" t="n">
-        <v>4826.9</v>
+      <c r="D33" s="19" t="n">
+        <v>809.11</v>
       </c>
       <c r="E33" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="F33" s="19" t="n">
-        <v>5671.46</v>
+      <c r="F33" s="26" t="n">
+        <v>780.7</v>
       </c>
       <c r="G33" s="10" t="inlineStr">
         <is>
@@ -3518,7 +3714,7 @@
         </is>
       </c>
       <c r="H33" s="19" t="n">
-        <v>4847.27</v>
+        <v>784.31</v>
       </c>
       <c r="I33" s="10" t="inlineStr">
         <is>
@@ -3526,7 +3722,7 @@
         </is>
       </c>
       <c r="J33" s="19" t="n">
-        <v>4785.62</v>
+        <v>776.18</v>
       </c>
       <c r="K33" s="10" t="inlineStr">
         <is>
@@ -3534,15 +3730,15 @@
         </is>
       </c>
       <c r="L33" s="19" t="n">
-        <v>5398.03</v>
+        <v>778.94</v>
       </c>
       <c r="M33" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="N33" s="19" t="n">
-        <v>5648.26</v>
+      <c r="N33" s="26" t="n">
+        <v>776.4</v>
       </c>
       <c r="O33" s="10" t="inlineStr">
         <is>
@@ -3550,7 +3746,7 @@
         </is>
       </c>
       <c r="P33" s="19" t="n">
-        <v>5318.08</v>
+        <v>764.87</v>
       </c>
       <c r="Q33" s="10" t="inlineStr">
         <is>
@@ -3558,19 +3754,25 @@
         </is>
       </c>
       <c r="R33" s="19" t="n">
-        <v>5206.57</v>
+        <v>747.46</v>
       </c>
       <c r="S33" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="T33" s="10" t="inlineStr">
-        <is>
-          <t>:</t>
-        </is>
+      <c r="T33" s="19" t="n">
+        <v>754.95</v>
       </c>
       <c r="U33" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V33" s="19" t="n">
+        <v>751.62</v>
+      </c>
+      <c r="W33" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -3582,8 +3784,8 @@
           <t>Poland</t>
         </is>
       </c>
-      <c r="B34" s="20" t="n">
-        <v>31369.67</v>
+      <c r="B34" s="30" t="n">
+        <v>7479.5</v>
       </c>
       <c r="C34" s="11" t="inlineStr">
         <is>
@@ -3591,31 +3793,31 @@
         </is>
       </c>
       <c r="D34" s="20" t="n">
-        <v>27481.72</v>
+        <v>7484.96</v>
       </c>
       <c r="E34" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="F34" s="20" t="n">
-        <v>29293.87</v>
+      <c r="F34" s="30" t="n">
+        <v>7511.8</v>
       </c>
       <c r="G34" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="H34" s="20" t="n">
-        <v>31331.01</v>
+      <c r="H34" s="30" t="n">
+        <v>7400.3</v>
       </c>
       <c r="I34" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J34" s="20" t="n">
-        <v>26281.55</v>
+      <c r="J34" s="30" t="n">
+        <v>7602.0</v>
       </c>
       <c r="K34" s="11" t="inlineStr">
         <is>
@@ -3623,15 +3825,15 @@
         </is>
       </c>
       <c r="L34" s="20" t="n">
-        <v>28450.92</v>
+        <v>7806.31</v>
       </c>
       <c r="M34" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="N34" s="30" t="n">
-        <v>35031.3</v>
+      <c r="N34" s="20" t="n">
+        <v>7891.43</v>
       </c>
       <c r="O34" s="11" t="inlineStr">
         <is>
@@ -3639,7 +3841,7 @@
         </is>
       </c>
       <c r="P34" s="20" t="n">
-        <v>33996.28</v>
+        <v>7466.68</v>
       </c>
       <c r="Q34" s="11" t="inlineStr">
         <is>
@@ -3647,21 +3849,27 @@
         </is>
       </c>
       <c r="R34" s="20" t="n">
-        <v>34616.03</v>
+        <v>7451.27</v>
       </c>
       <c r="S34" s="11" t="inlineStr">
         <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T34" s="20" t="n">
+        <v>7150.17</v>
+      </c>
+      <c r="U34" s="11" t="inlineStr">
+        <is>
           <t>e</t>
         </is>
       </c>
-      <c r="T34" s="11" t="inlineStr">
-        <is>
-          <t>:</t>
-        </is>
-      </c>
-      <c r="U34" s="11" t="inlineStr">
-        <is>
-          <t/>
+      <c r="V34" s="20" t="n">
+        <v>7122.27</v>
+      </c>
+      <c r="W34" s="11" t="inlineStr">
+        <is>
+          <t>e</t>
         </is>
       </c>
     </row>
@@ -3671,16 +3879,16 @@
           <t>Portugal</t>
         </is>
       </c>
-      <c r="B35" s="19" t="n">
-        <v>1346.36</v>
+      <c r="B35" s="26" t="n">
+        <v>315.1</v>
       </c>
       <c r="C35" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="D35" s="19" t="n">
-        <v>1252.36</v>
+      <c r="D35" s="26" t="n">
+        <v>303.2</v>
       </c>
       <c r="E35" s="10" t="inlineStr">
         <is>
@@ -3688,15 +3896,15 @@
         </is>
       </c>
       <c r="F35" s="19" t="n">
-        <v>1152.27</v>
+        <v>270.85</v>
       </c>
       <c r="G35" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="H35" s="26" t="n">
-        <v>1137.5</v>
+      <c r="H35" s="19" t="n">
+        <v>259.35</v>
       </c>
       <c r="I35" s="10" t="inlineStr">
         <is>
@@ -3704,7 +3912,7 @@
         </is>
       </c>
       <c r="J35" s="19" t="n">
-        <v>1116.32</v>
+        <v>238.55</v>
       </c>
       <c r="K35" s="10" t="inlineStr">
         <is>
@@ -3712,7 +3920,7 @@
         </is>
       </c>
       <c r="L35" s="19" t="n">
-        <v>1163.02</v>
+        <v>231.73</v>
       </c>
       <c r="M35" s="10" t="inlineStr">
         <is>
@@ -3720,15 +3928,15 @@
         </is>
       </c>
       <c r="N35" s="19" t="n">
-        <v>1055.08</v>
+        <v>224.32</v>
       </c>
       <c r="O35" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="P35" s="26" t="n">
-        <v>1127.7</v>
+      <c r="P35" s="19" t="n">
+        <v>215.83</v>
       </c>
       <c r="Q35" s="10" t="inlineStr">
         <is>
@@ -3736,19 +3944,27 @@
         </is>
       </c>
       <c r="R35" s="19" t="n">
-        <v>1021.14</v>
+        <v>209.24</v>
       </c>
       <c r="S35" s="10" t="inlineStr">
         <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T35" s="19" t="n">
+        <v>208.75</v>
+      </c>
+      <c r="U35" s="10" t="inlineStr">
+        <is>
           <t>p</t>
         </is>
       </c>
-      <c r="T35" s="19" t="n">
-        <v>979.91</v>
-      </c>
-      <c r="U35" s="10" t="inlineStr">
-        <is>
-          <t>p</t>
+      <c r="V35" s="19" t="n">
+        <v>194.13</v>
+      </c>
+      <c r="W35" s="10" t="inlineStr">
+        <is>
+          <t/>
         </is>
       </c>
     </row>
@@ -3758,8 +3974,8 @@
           <t>Romania</t>
         </is>
       </c>
-      <c r="B36" s="20" t="n">
-        <v>22070.74</v>
+      <c r="B36" s="30" t="n">
+        <v>5421.8</v>
       </c>
       <c r="C36" s="11" t="inlineStr">
         <is>
@@ -3767,7 +3983,7 @@
         </is>
       </c>
       <c r="D36" s="20" t="n">
-        <v>19332.82</v>
+        <v>5443.97</v>
       </c>
       <c r="E36" s="11" t="inlineStr">
         <is>
@@ -3775,23 +3991,23 @@
         </is>
       </c>
       <c r="F36" s="20" t="n">
-        <v>21764.82</v>
+        <v>5471.19</v>
       </c>
       <c r="G36" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="H36" s="20" t="n">
-        <v>27138.88</v>
+      <c r="H36" s="30" t="n">
+        <v>5490.2</v>
       </c>
       <c r="I36" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J36" s="20" t="n">
-        <v>31553.28</v>
+      <c r="J36" s="30" t="n">
+        <v>5195.5</v>
       </c>
       <c r="K36" s="11" t="inlineStr">
         <is>
@@ -3799,7 +4015,7 @@
         </is>
       </c>
       <c r="L36" s="20" t="n">
-        <v>30412.43</v>
+        <v>5261.28</v>
       </c>
       <c r="M36" s="11" t="inlineStr">
         <is>
@@ -3807,7 +4023,7 @@
         </is>
       </c>
       <c r="N36" s="20" t="n">
-        <v>18153.71</v>
+        <v>5572.51</v>
       </c>
       <c r="O36" s="11" t="inlineStr">
         <is>
@@ -3815,7 +4031,7 @@
         </is>
       </c>
       <c r="P36" s="20" t="n">
-        <v>27791.26</v>
+        <v>5341.51</v>
       </c>
       <c r="Q36" s="11" t="inlineStr">
         <is>
@@ -3823,7 +4039,7 @@
         </is>
       </c>
       <c r="R36" s="20" t="n">
-        <v>19183.59</v>
+        <v>5356.95</v>
       </c>
       <c r="S36" s="11" t="inlineStr">
         <is>
@@ -3831,9 +4047,17 @@
         </is>
       </c>
       <c r="T36" s="20" t="n">
-        <v>22757.46</v>
+        <v>5331.92</v>
       </c>
       <c r="U36" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V36" s="20" t="n">
+        <v>5239.78</v>
+      </c>
+      <c r="W36" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -3846,7 +4070,7 @@
         </is>
       </c>
       <c r="B37" s="19" t="n">
-        <v>649.06</v>
+        <v>98.97</v>
       </c>
       <c r="C37" s="10" t="inlineStr">
         <is>
@@ -3854,7 +4078,7 @@
         </is>
       </c>
       <c r="D37" s="19" t="n">
-        <v>624.05</v>
+        <v>99.88</v>
       </c>
       <c r="E37" s="10" t="inlineStr">
         <is>
@@ -3862,7 +4086,7 @@
         </is>
       </c>
       <c r="F37" s="19" t="n">
-        <v>638.06</v>
+        <v>98.96</v>
       </c>
       <c r="G37" s="10" t="inlineStr">
         <is>
@@ -3870,7 +4094,7 @@
         </is>
       </c>
       <c r="H37" s="19" t="n">
-        <v>546.99</v>
+        <v>95.51</v>
       </c>
       <c r="I37" s="10" t="inlineStr">
         <is>
@@ -3878,7 +4102,7 @@
         </is>
       </c>
       <c r="J37" s="19" t="n">
-        <v>596.66</v>
+        <v>98.46</v>
       </c>
       <c r="K37" s="10" t="inlineStr">
         <is>
@@ -3886,7 +4110,7 @@
         </is>
       </c>
       <c r="L37" s="19" t="n">
-        <v>641.74</v>
+        <v>98.25</v>
       </c>
       <c r="M37" s="10" t="inlineStr">
         <is>
@@ -3894,15 +4118,15 @@
         </is>
       </c>
       <c r="N37" s="19" t="n">
-        <v>749.69</v>
+        <v>98.62</v>
       </c>
       <c r="O37" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="P37" s="19" t="n">
-        <v>700.55</v>
+      <c r="P37" s="26" t="n">
+        <v>101.5</v>
       </c>
       <c r="Q37" s="10" t="inlineStr">
         <is>
@@ -3910,19 +4134,27 @@
         </is>
       </c>
       <c r="R37" s="19" t="n">
-        <v>576.32</v>
+        <v>102.05</v>
       </c>
       <c r="S37" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="T37" s="10" t="inlineStr">
+      <c r="T37" s="19" t="n">
+        <v>103.58</v>
+      </c>
+      <c r="U37" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V37" s="10" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="U37" s="10" t="inlineStr">
+      <c r="W37" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -3935,7 +4167,7 @@
         </is>
       </c>
       <c r="B38" s="20" t="n">
-        <v>4708.34</v>
+        <v>759.84</v>
       </c>
       <c r="C38" s="11" t="inlineStr">
         <is>
@@ -3943,7 +4175,7 @@
         </is>
       </c>
       <c r="D38" s="20" t="n">
-        <v>3805.71</v>
+        <v>779.03</v>
       </c>
       <c r="E38" s="11" t="inlineStr">
         <is>
@@ -3951,7 +4183,7 @@
         </is>
       </c>
       <c r="F38" s="20" t="n">
-        <v>4847.85</v>
+        <v>749.22</v>
       </c>
       <c r="G38" s="11" t="inlineStr">
         <is>
@@ -3959,7 +4191,7 @@
         </is>
       </c>
       <c r="H38" s="20" t="n">
-        <v>3484.06</v>
+        <v>752.32</v>
       </c>
       <c r="I38" s="11" t="inlineStr">
         <is>
@@ -3967,7 +4199,7 @@
         </is>
       </c>
       <c r="J38" s="20" t="n">
-        <v>4037.76</v>
+        <v>717.47</v>
       </c>
       <c r="K38" s="11" t="inlineStr">
         <is>
@@ -3975,7 +4207,7 @@
         </is>
       </c>
       <c r="L38" s="20" t="n">
-        <v>4104.06</v>
+        <v>743.15</v>
       </c>
       <c r="M38" s="11" t="inlineStr">
         <is>
@@ -3983,7 +4215,7 @@
         </is>
       </c>
       <c r="N38" s="20" t="n">
-        <v>4580.88</v>
+        <v>769.12</v>
       </c>
       <c r="O38" s="11" t="inlineStr">
         <is>
@@ -3991,15 +4223,15 @@
         </is>
       </c>
       <c r="P38" s="20" t="n">
-        <v>4308.04</v>
+        <v>747.32</v>
       </c>
       <c r="Q38" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="R38" s="20" t="n">
-        <v>3271.46</v>
+      <c r="R38" s="30" t="n">
+        <v>717.7</v>
       </c>
       <c r="S38" s="11" t="inlineStr">
         <is>
@@ -4007,9 +4239,17 @@
         </is>
       </c>
       <c r="T38" s="20" t="n">
-        <v>4215.65</v>
+        <v>718.38</v>
       </c>
       <c r="U38" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V38" s="20" t="n">
+        <v>696.95</v>
+      </c>
+      <c r="W38" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -4022,31 +4262,31 @@
         </is>
       </c>
       <c r="B39" s="26" t="n">
-        <v>4180.6</v>
+        <v>1099.7</v>
       </c>
       <c r="C39" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="D39" s="19" t="n">
-        <v>3729.91</v>
+      <c r="D39" s="26" t="n">
+        <v>1119.0</v>
       </c>
       <c r="E39" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="F39" s="19" t="n">
-        <v>3609.38</v>
+      <c r="F39" s="26" t="n">
+        <v>1017.3</v>
       </c>
       <c r="G39" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="H39" s="19" t="n">
-        <v>3462.12</v>
+      <c r="H39" s="26" t="n">
+        <v>998.1</v>
       </c>
       <c r="I39" s="10" t="inlineStr">
         <is>
@@ -4054,31 +4294,31 @@
         </is>
       </c>
       <c r="J39" s="19" t="n">
-        <v>2768.19</v>
+        <v>864.53</v>
       </c>
       <c r="K39" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="L39" s="19" t="n">
-        <v>4035.19</v>
+      <c r="L39" s="26" t="n">
+        <v>906.8</v>
       </c>
       <c r="M39" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="N39" s="19" t="n">
-        <v>3415.79</v>
+      <c r="N39" s="26" t="n">
+        <v>946.5</v>
       </c>
       <c r="O39" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="P39" s="19" t="n">
-        <v>2648.69</v>
+      <c r="P39" s="26" t="n">
+        <v>951.5</v>
       </c>
       <c r="Q39" s="10" t="inlineStr">
         <is>
@@ -4086,17 +4326,25 @@
         </is>
       </c>
       <c r="R39" s="19" t="n">
-        <v>3683.93</v>
+        <v>953.82</v>
       </c>
       <c r="S39" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="T39" s="26" t="n">
-        <v>3092.2</v>
+      <c r="T39" s="19" t="n">
+        <v>977.01</v>
       </c>
       <c r="U39" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V39" s="26" t="n">
+        <v>942.3</v>
+      </c>
+      <c r="W39" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -4108,32 +4356,32 @@
           <t>Sweden</t>
         </is>
       </c>
-      <c r="B40" s="30" t="n">
-        <v>5782.5</v>
+      <c r="B40" s="20" t="n">
+        <v>974.41</v>
       </c>
       <c r="C40" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="D40" s="30" t="n">
-        <v>6168.8</v>
+      <c r="D40" s="20" t="n">
+        <v>1023.64</v>
       </c>
       <c r="E40" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="F40" s="30" t="n">
-        <v>5480.5</v>
+      <c r="F40" s="20" t="n">
+        <v>1019.31</v>
       </c>
       <c r="G40" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="H40" s="30" t="n">
-        <v>5958.4</v>
+      <c r="H40" s="20" t="n">
+        <v>1004.68</v>
       </c>
       <c r="I40" s="11" t="inlineStr">
         <is>
@@ -4141,49 +4389,57 @@
         </is>
       </c>
       <c r="J40" s="30" t="n">
-        <v>3260.1</v>
+        <v>993.1</v>
       </c>
       <c r="K40" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="L40" s="30" t="n">
-        <v>6147.7</v>
+      <c r="L40" s="20" t="n">
+        <v>922.11</v>
       </c>
       <c r="M40" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="N40" s="30" t="n">
-        <v>5954.5</v>
+      <c r="N40" s="20" t="n">
+        <v>977.05</v>
       </c>
       <c r="O40" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="P40" s="30" t="n">
-        <v>4980.3</v>
+      <c r="P40" s="20" t="n">
+        <v>993.34</v>
       </c>
       <c r="Q40" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="R40" s="30" t="n">
-        <v>5820.4</v>
+      <c r="R40" s="20" t="n">
+        <v>983.34</v>
       </c>
       <c r="S40" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="T40" s="30" t="n">
-        <v>4949.0</v>
+      <c r="T40" s="20" t="n">
+        <v>953.34</v>
       </c>
       <c r="U40" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V40" s="20" t="n">
+        <v>932.47</v>
+      </c>
+      <c r="W40" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -4216,7 +4472,7 @@
         </is>
       </c>
       <c r="F41" s="26" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="G41" s="10" t="inlineStr">
         <is>
@@ -4224,57 +4480,65 @@
         </is>
       </c>
       <c r="H41" s="26" t="n">
-        <v>8.0</v>
+        <v>2.0</v>
       </c>
       <c r="I41" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J41" s="19" t="n">
-        <v>3.95</v>
+      <c r="J41" s="26" t="n">
+        <v>2.0</v>
       </c>
       <c r="K41" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="L41" s="19" t="n">
-        <v>4.94</v>
+      <c r="L41" s="26" t="n">
+        <v>1.5</v>
       </c>
       <c r="M41" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="N41" s="19" t="n">
-        <v>7.22</v>
+      <c r="N41" s="26" t="n">
+        <v>2.0</v>
       </c>
       <c r="O41" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="P41" s="19" t="n">
-        <v>7.41</v>
+      <c r="P41" s="26" t="n">
+        <v>2.8</v>
       </c>
       <c r="Q41" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="R41" s="19" t="n">
-        <v>9.29</v>
+      <c r="R41" s="26" t="n">
+        <v>2.6</v>
       </c>
       <c r="S41" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="T41" s="26" t="n">
-        <v>8.9</v>
+      <c r="T41" s="19" t="n">
+        <v>3.16</v>
       </c>
       <c r="U41" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V41" s="19" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="W41" s="10" t="inlineStr">
         <is>
           <t>e</t>
         </is>
@@ -4287,23 +4551,23 @@
         </is>
       </c>
       <c r="B42" s="30" t="n">
-        <v>1223.7</v>
+        <v>286.0</v>
       </c>
       <c r="C42" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="D42" s="20" t="n">
-        <v>1342.11</v>
+      <c r="D42" s="30" t="n">
+        <v>283.7</v>
       </c>
       <c r="E42" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="F42" s="20" t="n">
-        <v>1310.58</v>
+      <c r="F42" s="30" t="n">
+        <v>282.7</v>
       </c>
       <c r="G42" s="11" t="inlineStr">
         <is>
@@ -4311,15 +4575,15 @@
         </is>
       </c>
       <c r="H42" s="20" t="n">
-        <v>1292.08</v>
+        <v>285.05</v>
       </c>
       <c r="I42" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J42" s="30" t="n">
-        <v>734.4</v>
+      <c r="J42" s="20" t="n">
+        <v>286.79</v>
       </c>
       <c r="K42" s="11" t="inlineStr">
         <is>
@@ -4327,15 +4591,15 @@
         </is>
       </c>
       <c r="L42" s="20" t="n">
-        <v>1281.37</v>
+        <v>279.98</v>
       </c>
       <c r="M42" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="N42" s="30" t="n">
-        <v>1311.0</v>
+      <c r="N42" s="20" t="n">
+        <v>275.55</v>
       </c>
       <c r="O42" s="11" t="inlineStr">
         <is>
@@ -4343,29 +4607,37 @@
         </is>
       </c>
       <c r="P42" s="20" t="n">
-        <v>1170.88</v>
+        <v>280.22</v>
       </c>
       <c r="Q42" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="R42" s="11" t="inlineStr">
+      <c r="R42" s="30" t="n">
+        <v>283.5</v>
+      </c>
+      <c r="S42" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T42" s="11" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="S42" s="11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="T42" s="11" t="inlineStr">
+      <c r="U42" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V42" s="11" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="U42" s="11" t="inlineStr">
+      <c r="W42" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -4377,32 +4649,38 @@
           <t>Switzerland</t>
         </is>
       </c>
-      <c r="B43" s="19" t="n">
-        <v>974.63</v>
+      <c r="B43" s="10" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
       </c>
       <c r="C43" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="D43" s="19" t="n">
-        <v>901.75</v>
+      <c r="D43" s="10" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
       </c>
       <c r="E43" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="F43" s="19" t="n">
-        <v>752.06</v>
+      <c r="F43" s="10" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
       </c>
       <c r="G43" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="H43" s="19" t="n">
-        <v>986.72</v>
+      <c r="H43" s="26" t="n">
+        <v>144.1</v>
       </c>
       <c r="I43" s="10" t="inlineStr">
         <is>
@@ -4410,7 +4688,7 @@
         </is>
       </c>
       <c r="J43" s="19" t="n">
-        <v>891.58</v>
+        <v>143.32</v>
       </c>
       <c r="K43" s="10" t="inlineStr">
         <is>
@@ -4418,15 +4696,15 @@
         </is>
       </c>
       <c r="L43" s="19" t="n">
-        <v>942.73</v>
+        <v>141.73</v>
       </c>
       <c r="M43" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="N43" s="26" t="n">
-        <v>1021.3</v>
+      <c r="N43" s="19" t="n">
+        <v>141.45</v>
       </c>
       <c r="O43" s="10" t="inlineStr">
         <is>
@@ -4434,7 +4712,7 @@
         </is>
       </c>
       <c r="P43" s="19" t="n">
-        <v>791.47</v>
+        <v>144.54</v>
       </c>
       <c r="Q43" s="10" t="inlineStr">
         <is>
@@ -4442,19 +4720,27 @@
         </is>
       </c>
       <c r="R43" s="19" t="n">
-        <v>874.19</v>
+        <v>141.68</v>
       </c>
       <c r="S43" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="T43" s="10" t="inlineStr">
+      <c r="T43" s="19" t="n">
+        <v>141.95</v>
+      </c>
+      <c r="U43" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V43" s="10" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="U43" s="10" t="inlineStr">
+      <c r="W43" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -4467,47 +4753,49 @@
         </is>
       </c>
       <c r="B44" s="20" t="n">
-        <v>24382.41</v>
+        <v>3034.62</v>
       </c>
       <c r="C44" s="11" t="inlineStr">
         <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="D44" s="20" t="n">
-        <v>24591.19</v>
+          <t/>
+        </is>
+      </c>
+      <c r="D44" s="11" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
       </c>
       <c r="E44" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="F44" s="20" t="n">
-        <v>21710.58</v>
+      <c r="F44" s="30" t="n">
+        <v>3099.0</v>
       </c>
       <c r="G44" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="H44" s="20" t="n">
-        <v>22733.55</v>
+      <c r="H44" s="30" t="n">
+        <v>3128.0</v>
       </c>
       <c r="I44" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J44" s="20" t="n">
-        <v>20839.83</v>
+      <c r="J44" s="30" t="n">
+        <v>3181.0</v>
       </c>
       <c r="K44" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="L44" s="20" t="n">
-        <v>25219.86</v>
+      <c r="L44" s="30" t="n">
+        <v>3105.8</v>
       </c>
       <c r="M44" s="11" t="inlineStr">
         <is>
@@ -4515,39 +4803,47 @@
         </is>
       </c>
       <c r="N44" s="20" t="n">
-        <v>19469.45</v>
+        <v>3210.86</v>
       </c>
       <c r="O44" s="11" t="inlineStr">
         <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P44" s="20" t="n">
+        <v>3093.38</v>
+      </c>
+      <c r="Q44" s="11" t="inlineStr">
+        <is>
           <t>p</t>
         </is>
       </c>
-      <c r="P44" s="11" t="inlineStr">
+      <c r="R44" s="11" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="Q44" s="11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="R44" s="11" t="inlineStr">
+      <c r="S44" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="T44" s="11" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="S44" s="11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="T44" s="11" t="inlineStr">
+      <c r="U44" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V44" s="11" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="U44" s="11" t="inlineStr">
+      <c r="W44" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -4559,8 +4855,8 @@
           <t>Bosnia and Herzegovina</t>
         </is>
       </c>
-      <c r="B45" s="19" t="n">
-        <v>1094.66</v>
+      <c r="B45" s="26" t="n">
+        <v>304.9</v>
       </c>
       <c r="C45" s="10" t="inlineStr">
         <is>
@@ -4568,7 +4864,7 @@
         </is>
       </c>
       <c r="D45" s="19" t="n">
-        <v>1150.87</v>
+        <v>290.08</v>
       </c>
       <c r="E45" s="10" t="inlineStr">
         <is>
@@ -4576,7 +4872,7 @@
         </is>
       </c>
       <c r="F45" s="19" t="n">
-        <v>1677.52</v>
+        <v>301.57</v>
       </c>
       <c r="G45" s="10" t="inlineStr">
         <is>
@@ -4584,15 +4880,15 @@
         </is>
       </c>
       <c r="H45" s="19" t="n">
-        <v>1176.89</v>
+        <v>313.59</v>
       </c>
       <c r="I45" s="10" t="inlineStr">
         <is>
           <t>e</t>
         </is>
       </c>
-      <c r="J45" s="26" t="n">
-        <v>1764.1</v>
+      <c r="J45" s="19" t="n">
+        <v>313.98</v>
       </c>
       <c r="K45" s="10" t="inlineStr">
         <is>
@@ -4600,7 +4896,7 @@
         </is>
       </c>
       <c r="L45" s="19" t="n">
-        <v>1685.56</v>
+        <v>317.78</v>
       </c>
       <c r="M45" s="10" t="inlineStr">
         <is>
@@ -4608,7 +4904,7 @@
         </is>
       </c>
       <c r="N45" s="19" t="n">
-        <v>1966.78</v>
+        <v>311.24</v>
       </c>
       <c r="O45" s="10" t="inlineStr">
         <is>
@@ -4616,29 +4912,37 @@
         </is>
       </c>
       <c r="P45" s="19" t="n">
-        <v>1425.13</v>
+        <v>321.32</v>
       </c>
       <c r="Q45" s="10" t="inlineStr">
         <is>
           <t>e</t>
         </is>
       </c>
-      <c r="R45" s="10" t="inlineStr">
+      <c r="R45" s="19" t="n">
+        <v>317.64</v>
+      </c>
+      <c r="S45" s="10" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="T45" s="10" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="S45" s="10" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="T45" s="10" t="inlineStr">
+      <c r="U45" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V45" s="10" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="U45" s="10" t="inlineStr">
+      <c r="W45" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -4651,7 +4955,7 @@
         </is>
       </c>
       <c r="B46" s="20" t="n">
-        <v>8.01</v>
+        <v>2.15</v>
       </c>
       <c r="C46" s="11" t="inlineStr">
         <is>
@@ -4659,77 +4963,85 @@
         </is>
       </c>
       <c r="D46" s="20" t="n">
-        <v>7.09</v>
+        <v>2.36</v>
       </c>
       <c r="E46" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="F46" s="20" t="n">
-        <v>7.69</v>
+      <c r="F46" s="30" t="n">
+        <v>2.3</v>
       </c>
       <c r="G46" s="11" t="inlineStr">
         <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H46" s="20" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="I46" s="11" t="inlineStr">
+        <is>
           <t>p</t>
         </is>
       </c>
-      <c r="H46" s="20" t="n">
-        <v>7.87</v>
-      </c>
-      <c r="I46" s="11" t="inlineStr">
+      <c r="J46" s="20" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="K46" s="11" t="inlineStr">
         <is>
           <t>p</t>
         </is>
       </c>
-      <c r="J46" s="20" t="n">
-        <v>8.02</v>
-      </c>
-      <c r="K46" s="11" t="inlineStr">
+      <c r="L46" s="20" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="M46" s="11" t="inlineStr">
         <is>
           <t>p</t>
         </is>
       </c>
-      <c r="L46" s="20" t="n">
-        <v>7.58</v>
-      </c>
-      <c r="M46" s="11" t="inlineStr">
+      <c r="N46" s="20" t="n">
+        <v>2.43</v>
+      </c>
+      <c r="O46" s="11" t="inlineStr">
         <is>
           <t>p</t>
         </is>
       </c>
-      <c r="N46" s="20" t="n">
-        <v>7.28</v>
-      </c>
-      <c r="O46" s="11" t="inlineStr">
+      <c r="P46" s="30" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="Q46" s="11" t="inlineStr">
         <is>
           <t>p</t>
         </is>
       </c>
-      <c r="P46" s="30" t="n">
-        <v>7.1</v>
-      </c>
-      <c r="Q46" s="11" t="inlineStr">
+      <c r="R46" s="20" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="S46" s="11" t="inlineStr">
         <is>
           <t>p</t>
         </is>
       </c>
-      <c r="R46" s="11" t="inlineStr">
+      <c r="T46" s="11" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="S46" s="11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="T46" s="11" t="inlineStr">
+      <c r="U46" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V46" s="11" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="U46" s="11" t="inlineStr">
+      <c r="W46" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -4742,7 +5054,7 @@
         </is>
       </c>
       <c r="B47" s="19" t="n">
-        <v>636.48</v>
+        <v>167.08</v>
       </c>
       <c r="C47" s="10" t="inlineStr">
         <is>
@@ -4750,7 +5062,7 @@
         </is>
       </c>
       <c r="D47" s="19" t="n">
-        <v>489.44</v>
+        <v>162.12</v>
       </c>
       <c r="E47" s="10" t="inlineStr">
         <is>
@@ -4758,7 +5070,7 @@
         </is>
       </c>
       <c r="F47" s="19" t="n">
-        <v>648.36</v>
+        <v>159.63</v>
       </c>
       <c r="G47" s="10" t="inlineStr">
         <is>
@@ -4766,7 +5078,7 @@
         </is>
       </c>
       <c r="H47" s="19" t="n">
-        <v>452.91</v>
+        <v>167.68</v>
       </c>
       <c r="I47" s="10" t="inlineStr">
         <is>
@@ -4774,23 +5086,23 @@
         </is>
       </c>
       <c r="J47" s="19" t="n">
-        <v>605.26</v>
+        <v>160.78</v>
       </c>
       <c r="K47" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="L47" s="26" t="n">
-        <v>569.6</v>
+      <c r="L47" s="19" t="n">
+        <v>162.36</v>
       </c>
       <c r="M47" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="N47" s="26" t="n">
-        <v>585.5</v>
+      <c r="N47" s="19" t="n">
+        <v>160.22</v>
       </c>
       <c r="O47" s="10" t="inlineStr">
         <is>
@@ -4798,15 +5110,15 @@
         </is>
       </c>
       <c r="P47" s="19" t="n">
-        <v>568.88</v>
+        <v>159.45</v>
       </c>
       <c r="Q47" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="R47" s="26" t="n">
-        <v>548.4</v>
+      <c r="R47" s="19" t="n">
+        <v>161.47</v>
       </c>
       <c r="S47" s="10" t="inlineStr">
         <is>
@@ -4814,9 +5126,17 @@
         </is>
       </c>
       <c r="T47" s="19" t="n">
-        <v>577.97</v>
+        <v>159.03</v>
       </c>
       <c r="U47" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V47" s="19" t="n">
+        <v>160.81</v>
+      </c>
+      <c r="W47" s="10" t="inlineStr">
         <is>
           <t>e</t>
         </is>
@@ -4828,8 +5148,10 @@
           <t>Albania</t>
         </is>
       </c>
-      <c r="B48" s="30" t="n">
-        <v>700.0</v>
+      <c r="B48" s="11" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
       </c>
       <c r="C48" s="11" t="inlineStr">
         <is>
@@ -4837,7 +5159,7 @@
         </is>
       </c>
       <c r="D48" s="30" t="n">
-        <v>695.5</v>
+        <v>143.1</v>
       </c>
       <c r="E48" s="11" t="inlineStr">
         <is>
@@ -4845,33 +5167,33 @@
         </is>
       </c>
       <c r="F48" s="30" t="n">
-        <v>698.4</v>
+        <v>142.6</v>
       </c>
       <c r="G48" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="H48" s="11" t="inlineStr">
+      <c r="H48" s="30" t="n">
+        <v>148.0</v>
+      </c>
+      <c r="I48" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J48" s="11" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="I48" s="11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="J48" s="30" t="n">
-        <v>678.2</v>
-      </c>
       <c r="K48" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
       <c r="L48" s="30" t="n">
-        <v>666.1</v>
+        <v>140.1</v>
       </c>
       <c r="M48" s="11" t="inlineStr">
         <is>
@@ -4879,15 +5201,15 @@
         </is>
       </c>
       <c r="N48" s="30" t="n">
-        <v>684.0</v>
+        <v>132.2</v>
       </c>
       <c r="O48" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="P48" s="30" t="n">
-        <v>691.4</v>
+      <c r="P48" s="20" t="n">
+        <v>131.26</v>
       </c>
       <c r="Q48" s="11" t="inlineStr">
         <is>
@@ -4895,19 +5217,27 @@
         </is>
       </c>
       <c r="R48" s="30" t="n">
-        <v>690.9</v>
+        <v>134.3</v>
       </c>
       <c r="S48" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="T48" s="11" t="inlineStr">
+      <c r="T48" s="30" t="n">
+        <v>132.8</v>
+      </c>
+      <c r="U48" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V48" s="11" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="U48" s="11" t="inlineStr">
+      <c r="W48" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -4920,7 +5250,7 @@
         </is>
       </c>
       <c r="B49" s="19" t="n">
-        <v>10848.32</v>
+        <v>1758.37</v>
       </c>
       <c r="C49" s="10" t="inlineStr">
         <is>
@@ -4928,15 +5258,15 @@
         </is>
       </c>
       <c r="D49" s="19" t="n">
-        <v>8436.97</v>
+        <v>1816.68</v>
       </c>
       <c r="E49" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="F49" s="26" t="n">
-        <v>10868.0</v>
+      <c r="F49" s="19" t="n">
+        <v>1759.45</v>
       </c>
       <c r="G49" s="10" t="inlineStr">
         <is>
@@ -4944,15 +5274,15 @@
         </is>
       </c>
       <c r="H49" s="26" t="n">
-        <v>6793.3</v>
+        <v>1758.0</v>
       </c>
       <c r="I49" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J49" s="19" t="n">
-        <v>10529.06</v>
+      <c r="J49" s="26" t="n">
+        <v>1709.9</v>
       </c>
       <c r="K49" s="10" t="inlineStr">
         <is>
@@ -4960,7 +5290,7 @@
         </is>
       </c>
       <c r="L49" s="19" t="n">
-        <v>10436.43</v>
+        <v>1712.98</v>
       </c>
       <c r="M49" s="10" t="inlineStr">
         <is>
@@ -4968,7 +5298,7 @@
         </is>
       </c>
       <c r="N49" s="19" t="n">
-        <v>11447.57</v>
+        <v>1698.99</v>
       </c>
       <c r="O49" s="10" t="inlineStr">
         <is>
@@ -4976,7 +5306,7 @@
         </is>
       </c>
       <c r="P49" s="19" t="n">
-        <v>10236.39</v>
+        <v>1740.46</v>
       </c>
       <c r="Q49" s="10" t="inlineStr">
         <is>
@@ -4984,19 +5314,27 @@
         </is>
       </c>
       <c r="R49" s="19" t="n">
-        <v>8012.86</v>
+        <v>1770.19</v>
       </c>
       <c r="S49" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="T49" s="10" t="inlineStr">
+      <c r="T49" s="19" t="n">
+        <v>1724.74</v>
+      </c>
+      <c r="U49" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V49" s="10" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="U49" s="10" t="inlineStr">
+      <c r="W49" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -5009,7 +5347,7 @@
         </is>
       </c>
       <c r="B50" s="30" t="n">
-        <v>32382.0</v>
+        <v>11540.0</v>
       </c>
       <c r="C50" s="11" t="inlineStr">
         <is>
@@ -5017,75 +5355,83 @@
         </is>
       </c>
       <c r="D50" s="30" t="n">
-        <v>38637.0</v>
+        <v>11727.0</v>
       </c>
       <c r="E50" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="F50" s="20" t="n">
-        <v>35724.93</v>
+      <c r="F50" s="30" t="n">
+        <v>11713.0</v>
       </c>
       <c r="G50" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="H50" s="20" t="n">
-        <v>36598.79</v>
+      <c r="H50" s="30" t="n">
+        <v>11465.0</v>
       </c>
       <c r="I50" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J50" s="20" t="n">
-        <v>34705.75</v>
+      <c r="J50" s="30" t="n">
+        <v>11108.0</v>
       </c>
       <c r="K50" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="L50" s="20" t="n">
-        <v>35202.05</v>
+      <c r="L50" s="30" t="n">
+        <v>10899.0</v>
       </c>
       <c r="M50" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="N50" s="20" t="n">
-        <v>38050.79</v>
+      <c r="N50" s="30" t="n">
+        <v>10773.0</v>
       </c>
       <c r="O50" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="P50" s="20" t="n">
-        <v>32601.95</v>
+      <c r="P50" s="30" t="n">
+        <v>11144.0</v>
       </c>
       <c r="Q50" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="R50" s="20" t="n">
-        <v>39562.14</v>
+      <c r="R50" s="30" t="n">
+        <v>11136.0</v>
       </c>
       <c r="S50" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="T50" s="11" t="inlineStr">
+      <c r="T50" s="30" t="n">
+        <v>11198.0</v>
+      </c>
+      <c r="U50" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V50" s="11" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="U50" s="11" t="inlineStr">
+      <c r="W50" s="11" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -5098,15 +5444,15 @@
         </is>
       </c>
       <c r="B51" s="26" t="n">
-        <v>464.6</v>
+        <v>141.9</v>
       </c>
       <c r="C51" s="10" t="inlineStr">
         <is>
-          <t>e</t>
+          <t/>
         </is>
       </c>
       <c r="D51" s="26" t="n">
-        <v>443.6</v>
+        <v>132.9</v>
       </c>
       <c r="E51" s="10" t="inlineStr">
         <is>
@@ -5114,7 +5460,7 @@
         </is>
       </c>
       <c r="F51" s="26" t="n">
-        <v>562.9</v>
+        <v>134.9</v>
       </c>
       <c r="G51" s="10" t="inlineStr">
         <is>
@@ -5122,7 +5468,7 @@
         </is>
       </c>
       <c r="H51" s="26" t="n">
-        <v>477.9</v>
+        <v>134.6</v>
       </c>
       <c r="I51" s="10" t="inlineStr">
         <is>
@@ -5130,7 +5476,7 @@
         </is>
       </c>
       <c r="J51" s="26" t="n">
-        <v>441.8</v>
+        <v>120.7</v>
       </c>
       <c r="K51" s="10" t="inlineStr">
         <is>
@@ -5138,15 +5484,15 @@
         </is>
       </c>
       <c r="L51" s="26" t="n">
-        <v>459.4</v>
+        <v>123.9</v>
       </c>
       <c r="M51" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="N51" s="19" t="n">
-        <v>529.11</v>
+      <c r="N51" s="26" t="n">
+        <v>124.2</v>
       </c>
       <c r="O51" s="10" t="inlineStr">
         <is>
@@ -5154,7 +5500,7 @@
         </is>
       </c>
       <c r="P51" s="19" t="n">
-        <v>504.37</v>
+        <v>124.71</v>
       </c>
       <c r="Q51" s="10" t="inlineStr">
         <is>
@@ -5162,19 +5508,27 @@
         </is>
       </c>
       <c r="R51" s="19" t="n">
-        <v>518.72</v>
+        <v>124.48</v>
       </c>
       <c r="S51" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="T51" s="10" t="inlineStr">
+      <c r="T51" s="19" t="n">
+        <v>124.62</v>
+      </c>
+      <c r="U51" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V51" s="10" t="inlineStr">
         <is>
           <t>:</t>
         </is>
       </c>
-      <c r="U51" s="10" t="inlineStr">
+      <c r="W51" s="10" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -5243,7 +5597,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
@@ -5254,6 +5608,7 @@
     <mergeCell ref="P9:Q9"/>
     <mergeCell ref="R9:S9"/>
     <mergeCell ref="T9:U9"/>
+    <mergeCell ref="V9:W9"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>